<commit_message>
enable BSM1 simulation w/ ASM2d
</commit_message>
<xml_diff>
--- a/exposan/bsm1/data/initial_conditions_asm2d.xlsx
+++ b/exposan/bsm1/data/initial_conditions_asm2d.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yalin\Documents\Coding\EXPOsan\exposan\bsm1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\bsm1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D193846-9DF3-457E-BD5B-3629B51B2251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B59048-B8C7-43CC-801B-CFC309873720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="3214" windowWidth="24831" windowHeight="14495" xr2:uid="{32702723-0D76-4F6C-A6A7-E56FCE88CE75}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{32702723-0D76-4F6C-A6A7-E56FCE88CE75}"/>
   </bookViews>
   <sheets>
-    <sheet name="default" sheetId="5" r:id="rId1"/>
-    <sheet name="ss" sheetId="6" r:id="rId2"/>
+    <sheet name="obsolete" sheetId="5" r:id="rId1"/>
+    <sheet name="default" sheetId="7" r:id="rId2"/>
+    <sheet name="ss" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
   <si>
     <t>A1</t>
   </si>
@@ -125,6 +126,12 @@
   </si>
   <si>
     <t>X_PP</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>S_N2</t>
   </si>
 </sst>
 </file>
@@ -173,14 +180,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -205,9 +223,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -245,7 +263,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -351,7 +369,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,7 +511,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -503,20 +521,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E1BA80-9E8D-4883-B1AD-23C2415115BA}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="17" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -563,7 +581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -613,7 +631,7 @@
         <v>218.2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -663,7 +681,7 @@
         <v>11.93</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -713,7 +731,7 @@
         <v>58.03</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -763,7 +781,7 @@
         <v>64.02</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -813,7 +831,7 @@
         <v>218.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -844,7 +862,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -872,7 +890,7 @@
         <v>218.5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -910,7 +928,543 @@
       <c r="M9" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:N2">
+  <conditionalFormatting sqref="B1:N2 Q1">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5390B2-D129-4635-9B71-41C444BD0806}">
+  <dimension ref="A1:Q11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>30</v>
+      </c>
+      <c r="J2">
+        <f>6*12</f>
+        <v>72</v>
+      </c>
+      <c r="K2">
+        <v>1800</v>
+      </c>
+      <c r="L2">
+        <v>150</v>
+      </c>
+      <c r="M2">
+        <v>1900</v>
+      </c>
+      <c r="N2">
+        <v>250</v>
+      </c>
+      <c r="O2">
+        <v>70</v>
+      </c>
+      <c r="P2">
+        <v>7</v>
+      </c>
+      <c r="Q2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>30</v>
+      </c>
+      <c r="J3">
+        <v>72</v>
+      </c>
+      <c r="K3">
+        <v>1800</v>
+      </c>
+      <c r="L3">
+        <v>140</v>
+      </c>
+      <c r="M3">
+        <v>1900</v>
+      </c>
+      <c r="N3">
+        <v>250</v>
+      </c>
+      <c r="O3">
+        <v>70</v>
+      </c>
+      <c r="P3">
+        <v>18</v>
+      </c>
+      <c r="Q3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>30</v>
+      </c>
+      <c r="J4">
+        <v>60</v>
+      </c>
+      <c r="K4">
+        <v>1800</v>
+      </c>
+      <c r="L4">
+        <v>80</v>
+      </c>
+      <c r="M4">
+        <v>1900</v>
+      </c>
+      <c r="N4">
+        <v>250</v>
+      </c>
+      <c r="O4">
+        <v>70</v>
+      </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>30</v>
+      </c>
+      <c r="J5">
+        <v>60</v>
+      </c>
+      <c r="K5">
+        <v>1800</v>
+      </c>
+      <c r="L5">
+        <v>80</v>
+      </c>
+      <c r="M5">
+        <v>1900</v>
+      </c>
+      <c r="N5">
+        <v>250</v>
+      </c>
+      <c r="O5">
+        <v>70</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+      <c r="Q5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>48</v>
+      </c>
+      <c r="K6">
+        <v>1800</v>
+      </c>
+      <c r="L6">
+        <v>70</v>
+      </c>
+      <c r="M6">
+        <v>1900</v>
+      </c>
+      <c r="N6">
+        <v>250</v>
+      </c>
+      <c r="O6">
+        <v>70</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7">
+        <v>0.1</v>
+      </c>
+      <c r="I7">
+        <v>30</v>
+      </c>
+      <c r="J7">
+        <v>48</v>
+      </c>
+      <c r="K7">
+        <v>1800</v>
+      </c>
+      <c r="L7">
+        <v>60</v>
+      </c>
+      <c r="M7">
+        <v>1900</v>
+      </c>
+      <c r="N7">
+        <v>250</v>
+      </c>
+      <c r="O7">
+        <v>70</v>
+      </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
+        <v>0.1</v>
+      </c>
+      <c r="I8">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <v>48</v>
+      </c>
+      <c r="K8">
+        <v>1800</v>
+      </c>
+      <c r="L8">
+        <v>50</v>
+      </c>
+      <c r="M8">
+        <v>1900</v>
+      </c>
+      <c r="N8">
+        <v>250</v>
+      </c>
+      <c r="O8">
+        <v>70</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>30</v>
+      </c>
+      <c r="J9">
+        <f>7*12</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>200</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <v>200</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>70</v>
+      </c>
+      <c r="F11">
+        <v>400</v>
+      </c>
+      <c r="G11">
+        <v>400</v>
+      </c>
+      <c r="H11">
+        <v>400</v>
+      </c>
+      <c r="I11">
+        <v>400</v>
+      </c>
+      <c r="J11">
+        <v>400</v>
+      </c>
+      <c r="K11">
+        <v>4000</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:O1 R1:S1">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -919,24 +1473,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A69EC03-81D9-4A19-887C-E3BEAD631744}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="17" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -983,7 +1537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1033,7 +1587,7 @@
         <v>11.93</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1083,7 +1637,7 @@
         <v>38.82</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1133,7 +1687,7 @@
         <v>58.03</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1183,7 +1737,7 @@
         <v>64.02</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1233,7 +1787,7 @@
         <v>66.260000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1283,7 +1837,7 @@
         <v>67.31</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1333,7 +1887,7 @@
         <v>67.680000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1383,7 +1937,7 @@
         <v>67.650000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1433,7 +1987,7 @@
         <v>67.36</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1483,7 +2037,7 @@
         <v>66.92</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1533,7 +2087,7 @@
         <v>218.5</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1583,7 +2137,7 @@
         <v>218.2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1614,7 +2168,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1642,7 +2196,7 @@
         <v>218.5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>

</xml_diff>